<commit_message>
functional crud tests added
</commit_message>
<xml_diff>
--- a/Pool.xlsx
+++ b/Pool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAURICIO\Desktop\Nueva carpeta (7)\TF_Experimentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB351A3-06DF-4712-A5CC-EEB5C65DA859}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53FDE16-66E5-45C0-B637-6C36599115A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E665E48-A349-4275-8EBD-FC851F2C37D9}"/>
+    <workbookView xWindow="4575" yWindow="1005" windowWidth="15375" windowHeight="8910" xr2:uid="{2E665E48-A349-4275-8EBD-FC851F2C37D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t xml:space="preserve">Registro </t>
   </si>
@@ -100,6 +100,117 @@
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>Pruebas CRUD Clientes</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>masculino</t>
+  </si>
+  <si>
+    <t>premium</t>
+  </si>
+  <si>
+    <t>Nombre con numeros</t>
+  </si>
+  <si>
+    <t>Cedula con numeros</t>
+  </si>
+  <si>
+    <t>prueba1</t>
+  </si>
+  <si>
+    <t>Campo obligatorio faltante</t>
+  </si>
+  <si>
+    <t>Registro correcto</t>
+  </si>
+  <si>
+    <t>femenino</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Cedula solo letras</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Insertar</t>
+  </si>
+  <si>
+    <t>Mostrar</t>
+  </si>
+  <si>
+    <t>Cedula registrada</t>
+  </si>
+  <si>
+    <t>cedula1</t>
+  </si>
+  <si>
+    <t>cedula2</t>
+  </si>
+  <si>
+    <t>cedula3</t>
+  </si>
+  <si>
+    <t>Cedula no registrada</t>
+  </si>
+  <si>
+    <t>cedula4</t>
+  </si>
+  <si>
+    <t>se muestra</t>
+  </si>
+  <si>
+    <t>no se muestra</t>
+  </si>
+  <si>
+    <t>Cambiado</t>
+  </si>
+  <si>
+    <t>cedulacamb1</t>
+  </si>
+  <si>
+    <t>cambiado</t>
+  </si>
+  <si>
+    <t>Editar/Eliminar</t>
+  </si>
+  <si>
+    <t>ResultadoEliminar</t>
+  </si>
+  <si>
+    <t>ResultadoEditar</t>
+  </si>
+  <si>
+    <t>actualizó</t>
+  </si>
+  <si>
+    <t>se eliminó</t>
+  </si>
+  <si>
+    <t>nombre</t>
   </si>
 </sst>
 </file>
@@ -107,10 +218,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,19 +572,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E5BC87-4852-41DD-BEE3-F0820EE5719E}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -481,12 +601,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -500,7 +620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -514,7 +634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -528,12 +648,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -547,7 +667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -561,7 +681,238 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>